<commit_message>
Excel File fix minor
</commit_message>
<xml_diff>
--- a/ExcelFiles/Emails.xlsx
+++ b/ExcelFiles/Emails.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumars\IdeaProjects\ExcelReader\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh\Documents\GitHub\NewWeb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -845,9 +845,6 @@
     <t>R153</t>
   </si>
   <si>
-    <t>R154</t>
-  </si>
-  <si>
     <t>R155</t>
   </si>
   <si>
@@ -855,6 +852,9 @@
   </si>
   <si>
     <t>R157</t>
+  </si>
+  <si>
+    <t>R139</t>
   </si>
 </sst>
 </file>
@@ -1031,6 +1031,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1066,6 +1083,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1220,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2277,7 @@
         <v>35</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D73" s="1">
         <v>9999</v>
@@ -2397,7 +2431,7 @@
         <v>183</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D84" s="1">
         <v>9999</v>
@@ -2411,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D85" s="1">
         <v>9999</v>
@@ -2453,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D88" s="2">
         <v>9999</v>

</xml_diff>

<commit_message>
upload UI, message compose
</commit_message>
<xml_diff>
--- a/ExcelFiles/Emails.xlsx
+++ b/ExcelFiles/Emails.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurabh\Documents\GitHub\NewWeb\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AroraA\IdeaProjects\NewWeb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -848,22 +848,22 @@
     <t>R155</t>
   </si>
   <si>
-    <t>R156</t>
-  </si>
-  <si>
     <t>R157</t>
   </si>
   <si>
     <t>R139</t>
+  </si>
+  <si>
+    <t>R137</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -913,17 +913,17 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2277,7 @@
         <v>35</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D73" s="1">
         <v>9999</v>
@@ -2445,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D85" s="1">
         <v>9999</v>
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D88" s="2">
         <v>9999</v>

</xml_diff>

<commit_message>
Web Issues fixed, updated view details button
</commit_message>
<xml_diff>
--- a/ExcelFiles/Emails.xlsx
+++ b/ExcelFiles/Emails.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AroraA\IdeaProjects\NewWeb\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kumars\IdeaProjects\NewWeb\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -836,12 +836,6 @@
     <t>R150</t>
   </si>
   <si>
-    <t>R151</t>
-  </si>
-  <si>
-    <t>R152</t>
-  </si>
-  <si>
     <t>R153</t>
   </si>
   <si>
@@ -855,15 +849,21 @@
   </si>
   <si>
     <t>R137</t>
+  </si>
+  <si>
+    <t>R144</t>
+  </si>
+  <si>
+    <t>R145</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -913,17 +913,17 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,7 +1903,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="D46" s="1"/>
     </row>
@@ -1957,7 +1957,7 @@
         <v>77</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D50" s="1"/>
     </row>
@@ -2249,7 +2249,7 @@
         <v>39</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D71" s="1">
         <v>9999</v>
@@ -2277,7 +2277,7 @@
         <v>35</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D73" s="1">
         <v>9999</v>
@@ -2431,7 +2431,7 @@
         <v>183</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D84" s="1">
         <v>9999</v>
@@ -2445,7 +2445,7 @@
         <v>15</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D85" s="1">
         <v>9999</v>
@@ -2487,7 +2487,7 @@
         <v>9</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D88" s="2">
         <v>9999</v>

</xml_diff>